<commit_message>
viendo porque no agrego trade
</commit_message>
<xml_diff>
--- a/Trades.xlsx
+++ b/Trades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Limit Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Futures_bot_momentum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEC2CE1-7294-4EE1-8387-7A3853A8A051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE75C465-59A8-46DB-9E5E-417324AB490F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,9 +261,6 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="5" borderId="2" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -271,6 +268,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="4" borderId="2" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -292,27 +292,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -327,6 +306,42 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -343,31 +358,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -383,48 +383,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G32" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G32" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:G32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Side" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Quantity" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PNL" dataDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Commission" dataDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Symbol" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Side" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Quantity" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PNL" dataDxfId="19" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Commission" dataDxfId="18" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:G49" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:G49" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:G49" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Symbol" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Side" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Price" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Quantity" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="PNL" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Commission" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Symbol" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Side" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Type" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Price" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Quantity" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="PNL" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Commission" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{01C03075-B1DF-4393-86C3-32E146B08A02}" name="Table134" displayName="Table134" ref="A1:G49" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{01C03075-B1DF-4393-86C3-32E146B08A02}" name="Table134" displayName="Table134" ref="A1:G49" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G49" xr:uid="{01C03075-B1DF-4393-86C3-32E146B08A02}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{82D35446-1EED-4858-BC36-6F0C20C06185}" name="Symbol" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{16799848-B07D-4A97-9479-71D1B3DE1567}" name="Side" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{0BF040C8-3F32-4FF9-8AE7-FA245CBEBDF8}" name="Type" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{7A081B55-F03F-4B06-98F2-4F3075E08B55}" name="Price" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{DC174186-3506-47CA-A688-7BEE7E515883}" name="Quantity" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{D7B19A5F-A3DD-4694-B754-036A4467549F}" name="PNL" dataDxfId="12" dataCellStyle="Currency"/>
-    <tableColumn id="7" xr3:uid="{665D826B-E829-4122-B332-CC9AC777A0F6}" name="Commission" dataDxfId="13" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{82D35446-1EED-4858-BC36-6F0C20C06185}" name="Symbol" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{16799848-B07D-4A97-9479-71D1B3DE1567}" name="Side" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{0BF040C8-3F32-4FF9-8AE7-FA245CBEBDF8}" name="Type" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{7A081B55-F03F-4B06-98F2-4F3075E08B55}" name="Price" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{DC174186-3506-47CA-A688-7BEE7E515883}" name="Quantity" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D7B19A5F-A3DD-4694-B754-036A4467549F}" name="PNL" dataDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="7" xr3:uid="{665D826B-E829-4122-B332-CC9AC777A0F6}" name="Commission" dataDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -730,7 +730,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,10 +794,10 @@
       <c r="G2" s="5">
         <v>0.08</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -824,7 +824,7 @@
       <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="9">
         <f>ROUNDDOWN(COUNT(Table1[Quantity]) / 2, 0)</f>
         <v>1</v>
       </c>
@@ -894,7 +894,7 @@
       <c r="K10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <f>COUNTIFS(Table1[Side], "SELL", Table1[Type], "Closing Order", Table1[PNL], "&gt;0") / $L$9</f>
         <v>1</v>
       </c>
@@ -914,7 +914,7 @@
       <c r="K12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="11" t="e">
+      <c r="L12" s="10" t="e">
         <f>COUNTIFS(Table1[Side],"BUY", Table1[Type], "Closing Order", Table1[PNL],"&gt;0") / $L$11</f>
         <v>#DIV/0!</v>
       </c>
@@ -995,7 +995,7 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G9"/>
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1056,10 +1056,10 @@
       <c r="G2" s="5">
         <v>0.08</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1086,7 +1086,7 @@
       <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="9">
         <f>ROUNDDOWN(COUNT(Table13[Quantity]) / 2, 0)</f>
         <v>1</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="K10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <f>COUNTIFS(Table13[Side], "SELL", Table13[Type], "Closing Order", Table13[PNL], "&gt;0") / $L$9</f>
         <v>1</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="K12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="11" t="e">
+      <c r="L12" s="10" t="e">
         <f>COUNTIFS(Table13[Side],"BUY", Table13[Type], "Closing Order", Table13[PNL],"&gt;0") / $L$11</f>
         <v>#DIV/0!</v>
       </c>
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22EF89B7-CB28-4785-840E-25976190DA18}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1647,10 +1647,10 @@
       <c r="G2" s="5">
         <v>0.08</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1677,7 +1677,7 @@
       <c r="K3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="12">
+      <c r="L3" s="11">
         <f>ROUNDDOWN(COUNT(Table134[Quantity]) / 2, 0)</f>
         <v>1</v>
       </c>
@@ -1754,7 +1754,7 @@
       <c r="K10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="10">
         <f>COUNTIFS(Table134[Side], "SELL", Table134[Type], "Closing Order", Table134[PNL], "&gt;0") / $L$9</f>
         <v>1</v>
       </c>
@@ -1776,7 +1776,7 @@
       <c r="K12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L12" s="11" t="e">
+      <c r="L12" s="10" t="e">
         <f>COUNTIFS(Table134[Side],"BUY", Table134[Type], "Closing Order", Table134[PNL],"&gt;0") / $L$11</f>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
que append cualquier cosa a ve que apsa
</commit_message>
<xml_diff>
--- a/Trades.xlsx
+++ b/Trades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\Futures_bot_momentum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A8D863-04A3-4F02-B6EB-19096D566201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC3BEC9-29EE-4497-9F0E-ACAE5445E55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MATICUSDT" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>Symbol</t>
   </si>
@@ -88,15 +88,6 @@
   </si>
   <si>
     <t>Profitable Short %</t>
-  </si>
-  <si>
-    <t>MATICUSDT</t>
-  </si>
-  <si>
-    <t>SELL</t>
-  </si>
-  <si>
-    <t>Closing Order</t>
   </si>
 </sst>
 </file>
@@ -405,8 +396,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:G32" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="A1:G32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:G18" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:G18" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Symbol" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Side" dataDxfId="14"/>
@@ -735,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,50 +937,22 @@
       <c r="F32" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>18</v>
-      </c>
-      <c r="B38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38">
-        <v>1.381</v>
-      </c>
-      <c r="E38">
-        <v>146</v>
-      </c>
-      <c r="F38">
-        <v>0.876</v>
-      </c>
-      <c r="G38">
-        <v>8.0650399999999997E-2</v>
-      </c>
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39">
-        <v>1.381</v>
-      </c>
-      <c r="E39">
-        <v>146</v>
-      </c>
-      <c r="F39">
-        <v>0.876</v>
-      </c>
-      <c r="G39">
-        <v>8.0650399999999997E-2</v>
-      </c>
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1006,9 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1567,7 +1528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>